<commit_message>
Update DR# 711 USSC (Javelin DNA Pro Printers)_01_05_2022.xlsx
</commit_message>
<xml_diff>
--- a/DR# 711 USSC (Javelin DNA Pro Printers)_01_05_2022.xlsx
+++ b/DR# 711 USSC (Javelin DNA Pro Printers)_01_05_2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jaime Ponio IV\Documents\GitHub\Delivery-Receipt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1C85A30-17D8-4243-A5FA-53254218134F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05764FCC-8928-4051-8C79-D4D5B2412451}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -332,7 +332,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -379,22 +379,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -855,13 +858,13 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="50.25" customHeight="1">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="24"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
@@ -1077,13 +1080,13 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="50.25" customHeight="1">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="24"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
@@ -1270,7 +1273,7 @@
   <dimension ref="A2:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1298,13 +1301,13 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="50.25" customHeight="1">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="24"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
@@ -1357,25 +1360,25 @@
     </row>
     <row r="13" spans="1:9" ht="15.75" thickBot="1"/>
     <row r="14" spans="1:9" ht="31.5">
-      <c r="A14" s="25" t="s">
+      <c r="A14" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="26" t="s">
+      <c r="B14" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="27" t="s">
+      <c r="C14" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="27" t="s">
+      <c r="D14" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="E14" s="28" t="s">
+      <c r="E14" s="27" t="s">
         <v>5</v>
       </c>
       <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:9" ht="90">
-      <c r="A15" s="23" t="s">
+      <c r="A15" s="30" t="s">
         <v>23</v>
       </c>
       <c r="B15" s="22" t="s">
@@ -1387,7 +1390,7 @@
       <c r="D15" s="5">
         <v>5</v>
       </c>
-      <c r="E15" s="29">
+      <c r="E15" s="28">
         <v>44566</v>
       </c>
     </row>

</xml_diff>